<commit_message>
✨ feat : update file
</commit_message>
<xml_diff>
--- a/최종 풍력.xlsx
+++ b/최종 풍력.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorwh\Documents\test\we-meet\solar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorwh\Documents\GitHub\energy-estimator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1B39B3-B5D4-48E2-AE9C-C3E4CA6E7062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6C9EE2-5313-4BA1-8A5F-77C5DA373409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -221,7 +221,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>설비용량(kW)</t>
+    <t>설비용량</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -608,7 +608,7 @@
   <dimension ref="A1:AB181"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>